<commit_message>
Started the singly linked buffer evaluation
</commit_message>
<xml_diff>
--- a/Data Structures/linked_list/Singly Linked Buffer/MPMC_ALT.xlsx
+++ b/Data Structures/linked_list/Singly Linked Buffer/MPMC_ALT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="99">
   <si>
     <t xml:space="preserve"> Lockless Linked List Key Range 131072 (2^17)</t>
   </si>
@@ -283,6 +283,39 @@
   </si>
   <si>
     <t>Cube 128 Lockless</t>
+  </si>
+  <si>
+    <t>Stoker (32 Core) TASNP</t>
+  </si>
+  <si>
+    <t>Stoker TASNP</t>
+  </si>
+  <si>
+    <t>Pthread Mutex</t>
+  </si>
+  <si>
+    <t>Compare-and-swap</t>
+  </si>
+  <si>
+    <t>Test-and-set</t>
+  </si>
+  <si>
+    <t>Test-and-test-and-set</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Cache References</t>
+  </si>
+  <si>
+    <t>Cache Misses</t>
+  </si>
+  <si>
+    <t>Stalled Frontend Cycles</t>
+  </si>
+  <si>
+    <t>Lockless</t>
   </si>
 </sst>
 </file>
@@ -329,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -344,6 +377,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1405,11 +1440,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93725440"/>
-        <c:axId val="93727360"/>
+        <c:axId val="100012800"/>
+        <c:axId val="100014720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93725440"/>
+        <c:axId val="100012800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93727360"/>
+        <c:crossAx val="100014720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1446,7 +1481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93727360"/>
+        <c:axId val="100014720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1511,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93725440"/>
+        <c:crossAx val="100012800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1724,11 +1759,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39561472"/>
-        <c:axId val="39567744"/>
+        <c:axId val="100057088"/>
+        <c:axId val="100059008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39561472"/>
+        <c:axId val="100057088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39567744"/>
+        <c:crossAx val="100059008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1765,7 +1800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39567744"/>
+        <c:axId val="100059008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,7 +1830,891 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39561472"/>
+        <c:crossAx val="100057088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Singly Linked Buffer;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stoker; Best Performing Locks;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 128 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$15:$Y$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$16:$Y$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6109979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6003794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5753914</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4152627</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1452238</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1436272</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1206261</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1214998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) CAS lock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$15:$Y$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$17:$Y$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6006727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6013943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4368538</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4437876</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5997921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2985472</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3082779</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3150207</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$15:$Y$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$19:$Y$19</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6013591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8758255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4284720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8826226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4317215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4381121</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4448454</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6091243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$R$15:$Y$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$20:$Y$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4985510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4967422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3998237</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4061422</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4100502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4119303</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6174103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4358686</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="49769856"/>
+        <c:axId val="49800704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="49769856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49800704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49800704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49769856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Singly Linked Buffer;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stoker; Best Performing Locks;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 128 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AD$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AE$15:$AL$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AE$16:$AL$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6109979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6003794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5753914</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4152627</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1452238</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1436272</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1206261</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1214998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AD$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AE$15:$AL$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AE$18:$AL$18</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6013591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8758255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4284720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8826226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4317215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4381121</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4448454</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6091243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AD$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker 128 Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AE$15:$AL$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AE$20:$AL$20</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6157503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5291860</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5013554</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3595375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2736400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2624770</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2868725</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1490187</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="49408256"/>
+        <c:axId val="49410432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="49408256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49410432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49410432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49408256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1827,10 +2746,10 @@
       <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1857,10 +2776,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>4764</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1876,6 +2795,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2171,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:O409"/>
+  <dimension ref="A6:AL409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="Q7" workbookViewId="0">
+      <selection activeCell="AD41" sqref="AD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,9 +3168,12 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
+    <col min="30" max="30" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2197,7 +3183,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>47</v>
       </c>
@@ -2210,7 +3196,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -2236,7 +3222,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2265,7 +3251,7 @@
         <v>1031046</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -2294,7 +3280,7 @@
         <v>4487703</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2323,7 +3309,7 @@
         <v>666084</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2352,7 +3338,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2381,8 +3367,56 @@
         <v>7346657</v>
       </c>
       <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>4</v>
+      </c>
+      <c r="U15">
+        <v>8</v>
+      </c>
+      <c r="V15">
+        <v>16</v>
+      </c>
+      <c r="W15">
+        <v>32</v>
+      </c>
+      <c r="X15">
+        <v>64</v>
+      </c>
+      <c r="Y15">
+        <v>128</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>2</v>
+      </c>
+      <c r="AG15">
+        <v>4</v>
+      </c>
+      <c r="AH15">
+        <v>8</v>
+      </c>
+      <c r="AI15">
+        <v>16</v>
+      </c>
+      <c r="AJ15">
+        <v>32</v>
+      </c>
+      <c r="AK15">
+        <v>64</v>
+      </c>
+      <c r="AL15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2410,8 +3444,62 @@
       <c r="I16" s="6">
         <v>29313</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>49</v>
+      </c>
+      <c r="R16" s="6">
+        <v>6109979</v>
+      </c>
+      <c r="S16" s="6">
+        <v>6003794</v>
+      </c>
+      <c r="T16" s="6">
+        <v>5753914</v>
+      </c>
+      <c r="U16" s="6">
+        <v>4152627</v>
+      </c>
+      <c r="V16" s="6">
+        <v>1452238</v>
+      </c>
+      <c r="W16" s="6">
+        <v>1436272</v>
+      </c>
+      <c r="X16" s="6">
+        <v>1206261</v>
+      </c>
+      <c r="Y16" s="6">
+        <v>1214998</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE16" s="6">
+        <v>6109979</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>6003794</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>5753914</v>
+      </c>
+      <c r="AH16" s="6">
+        <v>4152627</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>1452238</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>1436272</v>
+      </c>
+      <c r="AK16" s="6">
+        <v>1206261</v>
+      </c>
+      <c r="AL16" s="6">
+        <v>1214998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2439,8 +3527,62 @@
       <c r="I17" s="6">
         <v>240599</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>48</v>
+      </c>
+      <c r="R17" s="6">
+        <v>6006727</v>
+      </c>
+      <c r="S17" s="6">
+        <v>6013943</v>
+      </c>
+      <c r="T17" s="6">
+        <v>4368538</v>
+      </c>
+      <c r="U17" s="6">
+        <v>4437876</v>
+      </c>
+      <c r="V17" s="6">
+        <v>5997921</v>
+      </c>
+      <c r="W17" s="6">
+        <v>2985472</v>
+      </c>
+      <c r="X17" s="6">
+        <v>3082779</v>
+      </c>
+      <c r="Y17" s="6">
+        <v>3150207</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE17" s="6">
+        <v>6006727</v>
+      </c>
+      <c r="AF17" s="6">
+        <v>6013943</v>
+      </c>
+      <c r="AG17" s="6">
+        <v>4368538</v>
+      </c>
+      <c r="AH17" s="6">
+        <v>4437876</v>
+      </c>
+      <c r="AI17" s="6">
+        <v>5997921</v>
+      </c>
+      <c r="AJ17" s="6">
+        <v>2985472</v>
+      </c>
+      <c r="AK17" s="6">
+        <v>3082779</v>
+      </c>
+      <c r="AL17" s="6">
+        <v>3150207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -2468,8 +3610,62 @@
       <c r="I18" s="6">
         <v>4435702</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>88</v>
+      </c>
+      <c r="R18" s="6">
+        <v>6011266</v>
+      </c>
+      <c r="S18" s="6">
+        <v>3506907</v>
+      </c>
+      <c r="T18" s="6">
+        <v>358469</v>
+      </c>
+      <c r="U18" s="6">
+        <v>230438</v>
+      </c>
+      <c r="V18" s="6">
+        <v>120121</v>
+      </c>
+      <c r="W18" s="6">
+        <v>59594</v>
+      </c>
+      <c r="X18" s="6">
+        <v>53271</v>
+      </c>
+      <c r="Y18" s="6">
+        <v>28299</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE18" s="6">
+        <v>6013591</v>
+      </c>
+      <c r="AF18" s="6">
+        <v>8758255</v>
+      </c>
+      <c r="AG18" s="6">
+        <v>4284720</v>
+      </c>
+      <c r="AH18" s="6">
+        <v>8826226</v>
+      </c>
+      <c r="AI18" s="6">
+        <v>4317215</v>
+      </c>
+      <c r="AJ18" s="6">
+        <v>4381121</v>
+      </c>
+      <c r="AK18" s="6">
+        <v>4448454</v>
+      </c>
+      <c r="AL18" s="6">
+        <v>6091243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2497,8 +3693,62 @@
       <c r="I19" s="6">
         <v>295064</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>55</v>
+      </c>
+      <c r="R19" s="6">
+        <v>6013591</v>
+      </c>
+      <c r="S19" s="6">
+        <v>8758255</v>
+      </c>
+      <c r="T19" s="6">
+        <v>4284720</v>
+      </c>
+      <c r="U19" s="6">
+        <v>8826226</v>
+      </c>
+      <c r="V19" s="6">
+        <v>4317215</v>
+      </c>
+      <c r="W19" s="6">
+        <v>4381121</v>
+      </c>
+      <c r="X19" s="6">
+        <v>4448454</v>
+      </c>
+      <c r="Y19" s="6">
+        <v>6091243</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE19">
+        <v>4985510</v>
+      </c>
+      <c r="AF19">
+        <v>4967422</v>
+      </c>
+      <c r="AG19">
+        <v>3998237</v>
+      </c>
+      <c r="AH19">
+        <v>4061422</v>
+      </c>
+      <c r="AI19">
+        <v>4100502</v>
+      </c>
+      <c r="AJ19">
+        <v>4119303</v>
+      </c>
+      <c r="AK19">
+        <v>6174103</v>
+      </c>
+      <c r="AL19">
+        <v>4358686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -2526,8 +3776,62 @@
       <c r="I20" s="6">
         <v>657259</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>52</v>
+      </c>
+      <c r="R20">
+        <v>4985510</v>
+      </c>
+      <c r="S20">
+        <v>4967422</v>
+      </c>
+      <c r="T20">
+        <v>3998237</v>
+      </c>
+      <c r="U20">
+        <v>4061422</v>
+      </c>
+      <c r="V20">
+        <v>4100502</v>
+      </c>
+      <c r="W20">
+        <v>4119303</v>
+      </c>
+      <c r="X20">
+        <v>6174103</v>
+      </c>
+      <c r="Y20">
+        <v>4358686</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE20" s="7">
+        <v>6157503</v>
+      </c>
+      <c r="AF20" s="7">
+        <v>5291860</v>
+      </c>
+      <c r="AG20" s="7">
+        <v>5013554</v>
+      </c>
+      <c r="AH20" s="7">
+        <v>3595375</v>
+      </c>
+      <c r="AI20" s="7">
+        <v>2736400</v>
+      </c>
+      <c r="AJ20" s="7">
+        <v>2624770</v>
+      </c>
+      <c r="AK20" s="7">
+        <v>2868725</v>
+      </c>
+      <c r="AL20" s="7">
+        <v>1490187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -2556,7 +3860,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -2585,7 +3889,7 @@
         <v>31279</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -2613,8 +3917,44 @@
       <c r="I23" s="6">
         <v>417348</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>84</v>
+      </c>
+      <c r="R23" s="10">
+        <v>2202585599063</v>
+      </c>
+      <c r="S23" t="s">
+        <v>3</v>
+      </c>
+      <c r="U23" t="s">
+        <v>18</v>
+      </c>
+      <c r="V23" s="10">
+        <v>91384491883</v>
+      </c>
+      <c r="W23" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z23" s="10">
+        <v>85860186583</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE23" s="10">
+        <v>942322908666</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2642,8 +3982,33 @@
       <c r="I24" s="6">
         <v>14115897</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R24" s="10">
+        <v>210887858402</v>
+      </c>
+      <c r="S24" t="s">
+        <v>4</v>
+      </c>
+      <c r="V24" s="10">
+        <v>82585421426</v>
+      </c>
+      <c r="W24" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z24" s="10">
+        <v>82462774107</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="10">
+        <v>105109197665</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -2671,8 +4036,33 @@
       <c r="I25" s="6">
         <v>7360144</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R25" s="10">
+        <v>632178469</v>
+      </c>
+      <c r="S25" t="s">
+        <v>5</v>
+      </c>
+      <c r="V25" s="10">
+        <v>80172267</v>
+      </c>
+      <c r="W25" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z25" s="10">
+        <v>91456490</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="10">
+        <v>699215767</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -2700,13 +4090,75 @@
       <c r="I26" s="6">
         <v>1113</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R26" s="10">
+        <v>292219852</v>
+      </c>
+      <c r="S26" t="s">
+        <v>6</v>
+      </c>
+      <c r="T26">
+        <v>44.434377859752225</v>
+      </c>
+      <c r="V26" s="10">
+        <v>71772629</v>
+      </c>
+      <c r="W26" t="s">
+        <v>6</v>
+      </c>
+      <c r="X26">
+        <v>91.31047094358334</v>
+      </c>
+      <c r="Z26" s="10">
+        <v>83326066</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB26">
+        <v>72.98154682712233</v>
+      </c>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="10">
+        <v>468130514</v>
+      </c>
+      <c r="AF26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG26">
+        <f>AE26/AE25*100</f>
+        <v>66.950794889612382</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R27" s="10">
+        <v>70017259408</v>
+      </c>
+      <c r="S27" t="s">
+        <v>7</v>
+      </c>
+      <c r="V27" s="10">
+        <v>16536998769</v>
+      </c>
+      <c r="W27" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="10">
+        <v>16685113624</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE27" s="10">
+        <v>28620956466</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -2734,8 +4186,45 @@
       <c r="I28" s="6">
         <v>3800070</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R28" s="10">
+        <v>79490726</v>
+      </c>
+      <c r="S28" t="s">
+        <v>8</v>
+      </c>
+      <c r="T28">
+        <v>8.4829484238065064E-2</v>
+      </c>
+      <c r="V28" s="10">
+        <v>9759767</v>
+      </c>
+      <c r="W28" t="s">
+        <v>8</v>
+      </c>
+      <c r="X28">
+        <v>2.6367329568261117E-2</v>
+      </c>
+      <c r="Z28" s="10">
+        <v>11109930</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB28">
+        <v>3.4478659030337672E-2</v>
+      </c>
+      <c r="AE28" s="10">
+        <v>95634737</v>
+      </c>
+      <c r="AF28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG28">
+        <f>AE28/AE27*100</f>
+        <v>0.33414235164924833</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2763,8 +4252,32 @@
       <c r="I29" s="6">
         <v>4446192</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R29" s="10">
+        <v>146237642275</v>
+      </c>
+      <c r="S29" t="s">
+        <v>9</v>
+      </c>
+      <c r="V29" s="10">
+        <v>7492998529</v>
+      </c>
+      <c r="W29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z29" s="10">
+        <v>7506143790</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE29" s="10">
+        <v>70168743533</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2792,8 +4305,32 @@
       <c r="I30" s="6">
         <v>2382859</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R30" s="10">
+        <v>1107224.669398</v>
+      </c>
+      <c r="S30" t="s">
+        <v>10</v>
+      </c>
+      <c r="V30" s="10">
+        <v>56886.674969</v>
+      </c>
+      <c r="W30" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z30" s="10">
+        <v>56981.005034000002</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE30" s="10">
+        <v>533364.89931200002</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -2821,8 +4358,32 @@
       <c r="I31" s="6">
         <v>4048673</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R31" s="10">
+        <v>1107211.2498389999</v>
+      </c>
+      <c r="S31" t="s">
+        <v>11</v>
+      </c>
+      <c r="V31" s="10">
+        <v>56886.886126999998</v>
+      </c>
+      <c r="W31" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z31" s="10">
+        <v>56981.141070999998</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE31" s="10">
+        <v>533357.16200600006</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -2850,8 +4411,45 @@
       <c r="I32" s="6">
         <v>7868681</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R32" s="10">
+        <v>2089119750384</v>
+      </c>
+      <c r="S32" t="s">
+        <v>15</v>
+      </c>
+      <c r="T32">
+        <v>93.917109487672334</v>
+      </c>
+      <c r="V32" s="10">
+        <v>56565317064</v>
+      </c>
+      <c r="W32" t="s">
+        <v>15</v>
+      </c>
+      <c r="X32">
+        <v>59.559950503294154</v>
+      </c>
+      <c r="Z32" s="10">
+        <v>51308018271</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB32">
+        <v>69.624266612618086</v>
+      </c>
+      <c r="AE32" s="10">
+        <v>887677025500</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG32">
+        <f>AE32/AE23*100</f>
+        <v>94.200938694851487</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2879,8 +4477,45 @@
       <c r="I33" s="6">
         <v>274279</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R33" s="10">
+        <v>1419933816951</v>
+      </c>
+      <c r="S33" t="s">
+        <v>16</v>
+      </c>
+      <c r="T33">
+        <v>63.468447074869474</v>
+      </c>
+      <c r="V33" s="10">
+        <v>44789627319</v>
+      </c>
+      <c r="W33" t="s">
+        <v>16</v>
+      </c>
+      <c r="X33">
+        <v>48.342952534878577</v>
+      </c>
+      <c r="Z33" s="10">
+        <v>41527600786</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB33">
+        <v>42.662589725996227</v>
+      </c>
+      <c r="AE33" s="10">
+        <v>653202788644</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG33">
+        <f>AE33/AE23*100</f>
+        <v>69.318360260253769</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2908,8 +4543,10 @@
       <c r="I34" s="6">
         <v>2949705</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R34" s="11"/>
+      <c r="V34" s="11"/>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2937,8 +4574,26 @@
       <c r="I35" s="6">
         <v>3045309</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q35" t="s">
+        <v>89</v>
+      </c>
+      <c r="R35" s="10">
+        <v>2676043396360</v>
+      </c>
+      <c r="S35" t="s">
+        <v>3</v>
+      </c>
+      <c r="U35" t="s">
+        <v>26</v>
+      </c>
+      <c r="V35" s="10">
+        <v>87830712750</v>
+      </c>
+      <c r="W35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -2966,8 +4621,20 @@
       <c r="I36" s="6">
         <v>4296401</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R36" s="10">
+        <v>32081013529</v>
+      </c>
+      <c r="S36" t="s">
+        <v>4</v>
+      </c>
+      <c r="V36" s="10">
+        <v>85136250591</v>
+      </c>
+      <c r="W36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -2995,8 +4662,35 @@
       <c r="I37" s="6">
         <v>3944918</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R37" s="10">
+        <v>268424082</v>
+      </c>
+      <c r="S37" t="s">
+        <v>5</v>
+      </c>
+      <c r="V37" s="10">
+        <v>98977343</v>
+      </c>
+      <c r="W37" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -3024,8 +4718,44 @@
       <c r="I38" s="7">
         <v>292</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R38" s="10">
+        <v>243361994</v>
+      </c>
+      <c r="S38" t="s">
+        <v>6</v>
+      </c>
+      <c r="T38">
+        <v>44.434377859752225</v>
+      </c>
+      <c r="V38" s="10">
+        <v>89435389</v>
+      </c>
+      <c r="W38" t="s">
+        <v>6</v>
+      </c>
+      <c r="X38">
+        <v>44.434377859752225</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE38" s="10">
+        <v>2202585599063</v>
+      </c>
+      <c r="AF38" s="10">
+        <v>632178469</v>
+      </c>
+      <c r="AG38" s="10">
+        <v>292219852</v>
+      </c>
+      <c r="AH38" s="10">
+        <v>2089119750384</v>
+      </c>
+      <c r="AI38" s="10">
+        <v>1419933816951</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -3037,8 +4767,38 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R39" s="10">
+        <v>6904877989</v>
+      </c>
+      <c r="S39" t="s">
+        <v>7</v>
+      </c>
+      <c r="V39" s="10">
+        <v>17129009371</v>
+      </c>
+      <c r="W39" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD39" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE39" s="10">
+        <v>91384491883</v>
+      </c>
+      <c r="AF39" s="10">
+        <v>80172267</v>
+      </c>
+      <c r="AG39" s="10">
+        <v>71772629</v>
+      </c>
+      <c r="AH39" s="10">
+        <v>56565317064</v>
+      </c>
+      <c r="AI39" s="10">
+        <v>44789627319</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -3066,8 +4826,44 @@
       <c r="I40" s="6">
         <v>120227</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R40" s="10">
+        <v>21338098</v>
+      </c>
+      <c r="S40" t="s">
+        <v>8</v>
+      </c>
+      <c r="T40">
+        <v>8.4829484238065064E-2</v>
+      </c>
+      <c r="V40" s="10">
+        <v>4662643</v>
+      </c>
+      <c r="W40" t="s">
+        <v>8</v>
+      </c>
+      <c r="X40">
+        <v>8.4829484238065064E-2</v>
+      </c>
+      <c r="AD40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE40" s="10">
+        <v>942322908666</v>
+      </c>
+      <c r="AF40" s="10">
+        <v>699215767</v>
+      </c>
+      <c r="AG40" s="10">
+        <v>468130514</v>
+      </c>
+      <c r="AH40" s="10">
+        <v>887677025500</v>
+      </c>
+      <c r="AI40" s="10">
+        <v>653202788644</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -3095,8 +4891,20 @@
       <c r="I41" s="6">
         <v>433174</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R41" s="10">
+        <v>170821202952</v>
+      </c>
+      <c r="S41" t="s">
+        <v>9</v>
+      </c>
+      <c r="V41" s="10">
+        <v>7488196515</v>
+      </c>
+      <c r="W41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -3124,8 +4932,20 @@
       <c r="I42" s="6">
         <v>4259875</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R42" s="10">
+        <v>1291907.611644</v>
+      </c>
+      <c r="S42" t="s">
+        <v>10</v>
+      </c>
+      <c r="V42" s="10">
+        <v>56936.811952999997</v>
+      </c>
+      <c r="W42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -3153,8 +4973,20 @@
       <c r="I43" s="6">
         <v>1004182</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R43" s="10">
+        <v>1291909.8097049999</v>
+      </c>
+      <c r="S43" t="s">
+        <v>11</v>
+      </c>
+      <c r="V43" s="10">
+        <v>56938.008996999997</v>
+      </c>
+      <c r="W43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -3182,8 +5014,26 @@
       <c r="I44" s="6">
         <v>4508441</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R44" s="10">
+        <v>2660562193137</v>
+      </c>
+      <c r="S44" t="s">
+        <v>15</v>
+      </c>
+      <c r="T44">
+        <v>93.917109487672334</v>
+      </c>
+      <c r="V44" s="10">
+        <v>52205906918</v>
+      </c>
+      <c r="W44" t="s">
+        <v>15</v>
+      </c>
+      <c r="X44">
+        <v>93.917109487672334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -3211,8 +5061,26 @@
       <c r="I45" s="6">
         <v>1020</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="R45" s="10">
+        <v>2593490453050</v>
+      </c>
+      <c r="S45" t="s">
+        <v>16</v>
+      </c>
+      <c r="T45">
+        <v>63.468447074869474</v>
+      </c>
+      <c r="V45" s="10">
+        <v>41937350076</v>
+      </c>
+      <c r="W45" t="s">
+        <v>16</v>
+      </c>
+      <c r="X45">
+        <v>63.468447074869474</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -3241,7 +5109,44 @@
         <v>126632</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R47" t="s">
+        <v>94</v>
+      </c>
+      <c r="S47" t="s">
+        <v>95</v>
+      </c>
+      <c r="T47" t="s">
+        <v>96</v>
+      </c>
+      <c r="U47" t="s">
+        <v>97</v>
+      </c>
+      <c r="V47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="Q48" t="s">
+        <v>90</v>
+      </c>
+      <c r="R48" s="10">
+        <v>2202585599063</v>
+      </c>
+      <c r="S48" s="10">
+        <v>632178469</v>
+      </c>
+      <c r="T48" s="10">
+        <v>292219852</v>
+      </c>
+      <c r="U48" s="10">
+        <v>2089119750384</v>
+      </c>
+      <c r="V48" s="10">
+        <v>1419933816951</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>2</v>
       </c>
@@ -3253,8 +5158,26 @@
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49" t="s">
+        <v>91</v>
+      </c>
+      <c r="R49" s="10">
+        <v>85860186583</v>
+      </c>
+      <c r="S49" s="10">
+        <v>91456490</v>
+      </c>
+      <c r="T49" s="10">
+        <v>83326066</v>
+      </c>
+      <c r="U49" s="10">
+        <v>51308018271</v>
+      </c>
+      <c r="V49" s="10">
+        <v>41527600786</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>1</v>
       </c>
@@ -3279,8 +5202,26 @@
       <c r="I50">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q50" t="s">
+        <v>92</v>
+      </c>
+      <c r="R50" s="10">
+        <v>87830712750</v>
+      </c>
+      <c r="S50" s="10">
+        <v>98977343</v>
+      </c>
+      <c r="T50" s="10">
+        <v>89435389</v>
+      </c>
+      <c r="U50" s="10">
+        <v>52205906918</v>
+      </c>
+      <c r="V50" s="10">
+        <v>41937350076</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>85</v>
       </c>
@@ -3308,8 +5249,26 @@
       <c r="I51" s="7">
         <v>1746792</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q51" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R51" s="10">
+        <v>91384491883</v>
+      </c>
+      <c r="S51" s="10">
+        <v>80172267</v>
+      </c>
+      <c r="T51" s="10">
+        <v>71772629</v>
+      </c>
+      <c r="U51" s="10">
+        <v>56565317064</v>
+      </c>
+      <c r="V51" s="10">
+        <v>44789627319</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>86</v>
       </c>
@@ -3338,7 +5297,7 @@
         <v>14041670</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>87</v>
       </c>
@@ -3367,18 +5326,18 @@
         <v>7659168</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>0</v>
       </c>
@@ -3391,7 +5350,7 @@
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>1</v>
       </c>
@@ -3417,7 +5376,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>41</v>
       </c>
@@ -3446,7 +5405,7 @@
         <v>1735253</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>42</v>
       </c>
@@ -3476,7 +5435,7 @@
       </c>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>43</v>
       </c>
@@ -3506,19 +5465,19 @@
       </c>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="1"/>
       <c r="E62" s="2"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="1"/>
       <c r="E63" s="2"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="1"/>
       <c r="E64" s="2"/>

</xml_diff>